<commit_message>
Implemented pg datatype differentiation. everything works except numerics and reals. could use some more fail safe logic if the data is wrong.
</commit_message>
<xml_diff>
--- a/test/datebool_test.xlsx
+++ b/test/datebool_test.xlsx
@@ -21,11 +21,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-407]dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;WAHR&quot;;&quot;WAHR&quot;;&quot;FALSCH&quot;"/>
-    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -93,7 +92,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -107,10 +106,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,40 +129,43 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.21"/>
-  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <v>34263</v>
       </c>
-      <c r="B1" s="2" t="b">
+      <c r="B1" s="1" t="n">
+        <v>34263</v>
+      </c>
+      <c r="C1" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>34602</v>
       </c>
-      <c r="B2" s="2" t="b">
+      <c r="B2" s="1" t="n">
+        <v>34602</v>
+      </c>
+      <c r="C2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>45437</v>
+        <v>45436</v>
       </c>
-      <c r="B3" s="2" t="b">
+      <c r="B3" s="1" t="n">
+        <v>45436</v>
+      </c>
+      <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>

</xml_diff>